<commit_message>
generated with Celerio v3.0.100 - http://www.springfuse.com/
</commit_message>
<xml_diff>
--- a/jpa2-backend/src/main/resources/excel/account.xlsx
+++ b/jpa2-backend/src/main/resources/excel/account.xlsx
@@ -137,6 +137,12 @@
     <t>${msg.getProperty('search_criteria')}</t>
   </si>
   <si>
+    <t>${msg.getProperty('search_full_text')}</t>
+  </si>
+  <si>
+    <t>${search_full_text}</t>
+  </si>
+  <si>
     <t>${username}</t>
   </si>
   <si>
@@ -173,16 +179,10 @@
     <t>${description}</t>
   </si>
   <si>
-    <t>${msg.getProperty('account_homeAddress')}</t>
-  </si>
-  <si>
-    <t>${homeAddress}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('Role')}</t>
-  </si>
-  <si>
-    <t>${roles}</t>
+    <t>${msg.getProperty('Security Roles')}</t>
+  </si>
+  <si>
+    <t>${securityRoles}</t>
   </si>
 </sst>
 </file>
@@ -681,88 +681,88 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" t="s">
         <v>47</v>
-      </c>
-      <c r="D11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
         <v>50</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
generated with Celerio v3.0.101 - http://www.springfuse.com/
</commit_message>
<xml_diff>
--- a/jpa2-backend/src/main/resources/excel/account.xlsx
+++ b/jpa2-backend/src/main/resources/excel/account.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
   <si>
     <t>${msg.getProperty('account_id')}</t>
   </si>
@@ -53,7 +53,7 @@
     <t>${msg.getProperty('account_civility')}</t>
   </si>
   <si>
-    <t>${account.civility}</t>
+    <t>${account.civility.label}</t>
   </si>
   <si>
     <t>${msg.getProperty('account_firstName')}</t>
@@ -80,10 +80,10 @@
     <t>${account.description}</t>
   </si>
   <si>
-    <t>${msg.getProperty('account_addressId')}</t>
-  </si>
-  <si>
-    <t>${account.addressId}</t>
+    <t>${msg.getProperty('account_homeAddress')}</t>
+  </si>
+  <si>
+    <t>${printer.print(account.homeAddress)}</t>
   </si>
   <si>
     <t>${msg.getProperty('account_creationDate')}</t>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>${description}</t>
+  </si>
+  <si>
+    <t>${homeAddress}</t>
   </si>
   <si>
     <t>${msg.getProperty('Security Roles')}</t>
@@ -770,10 +773,18 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
         <v>53</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
         <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generated with Celerio v3.0.102 - http://www.springfuse.com/
</commit_message>
<xml_diff>
--- a/jpa2-backend/src/main/resources/excel/account.xlsx
+++ b/jpa2-backend/src/main/resources/excel/account.xlsx
@@ -18,174 +18,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
-  <si>
-    <t>${msg.getProperty('account_id')}</t>
-  </si>
-  <si>
-    <t>${account.id}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('account_username')}</t>
-  </si>
-  <si>
-    <t>${account.username}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('account_password')}</t>
-  </si>
-  <si>
-    <t>${account.password}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('account_email')}</t>
-  </si>
-  <si>
-    <t>${account.email}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('account_isEnabled')}</t>
-  </si>
-  <si>
-    <t>${account.isEnabled}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('account_civility')}</t>
-  </si>
-  <si>
-    <t>${account.civility.label}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('account_firstName')}</t>
-  </si>
-  <si>
-    <t>${account.firstName}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('account_lastName')}</t>
-  </si>
-  <si>
-    <t>${account.lastName}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('account_birthDate')}</t>
-  </si>
-  <si>
-    <t>${account.birthDate}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('account_description')}</t>
-  </si>
-  <si>
-    <t>${account.description}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('account_homeAddress')}</t>
-  </si>
-  <si>
-    <t>${printer.print(account.homeAddress)}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('account_creationDate')}</t>
-  </si>
-  <si>
-    <t>${account.creationDate}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('account_creationAuthor')}</t>
-  </si>
-  <si>
-    <t>${account.creationAuthor}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('account_lastModificationDate')}</t>
-  </si>
-  <si>
-    <t>${account.lastModificationDate}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('account_lastModificationAuthor')}</t>
-  </si>
-  <si>
-    <t>${account.lastModificationAuthor}</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+  <si>
+    <t>${msg.getProperty('account_accountNumber')}</t>
+  </si>
+  <si>
+    <t>${account.accountNumber}</t>
+  </si>
+  <si>
+    <t>${msg.getProperty('account_name')}</t>
+  </si>
+  <si>
+    <t>${account.name}</t>
+  </si>
+  <si>
+    <t>${msg.getProperty('account_customer')}</t>
+  </si>
+  <si>
+    <t>${printer.print(account.customer)}</t>
+  </si>
+  <si>
+    <t>${msg.getProperty('search_date')}</t>
+  </si>
+  <si>
+    <t>${search_date}</t>
+  </si>
+  <si>
+    <t>${msg.getProperty('search_by')}</t>
+  </si>
+  <si>
+    <t>${search_by}</t>
+  </si>
+  <si>
+    <t>${msg.getProperty('search_nb_results')}</t>
+  </si>
+  <si>
+    <t>${search_nb_results}</t>
+  </si>
+  <si>
+    <t>${msg.getProperty('search_criteria')}</t>
+  </si>
+  <si>
+    <t>${msg.getProperty('account_transactions')}</t>
+  </si>
+  <si>
+    <t>${transaction}</t>
+  </si>
+  <si>
+    <t>${accountNumber}</t>
+  </si>
+  <si>
+    <t>${name}</t>
+  </si>
+  <si>
+    <t>${msg.getProperty('account_currency')}</t>
+  </si>
+  <si>
+    <t>${currency}</t>
+  </si>
+  <si>
+    <t>${customer}</t>
   </si>
   <si>
     <t>${msg.getProperty('account_version')}</t>
   </si>
   <si>
-    <t>${account.version}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('search_date')}</t>
-  </si>
-  <si>
-    <t>${search_date}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('search_by')}</t>
-  </si>
-  <si>
-    <t>${search_by}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('search_nb_results')}</t>
-  </si>
-  <si>
-    <t>${search_nb_results}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('search_criteria')}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('search_full_text')}</t>
-  </si>
-  <si>
-    <t>${search_full_text}</t>
-  </si>
-  <si>
-    <t>${username}</t>
-  </si>
-  <si>
-    <t>${password}</t>
-  </si>
-  <si>
-    <t>${email}</t>
-  </si>
-  <si>
-    <t>${isEnabled}</t>
-  </si>
-  <si>
-    <t>${civility}</t>
-  </si>
-  <si>
-    <t>${firstName}</t>
-  </si>
-  <si>
-    <t>${lastName}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('range_from')}</t>
-  </si>
-  <si>
-    <t>${birthDateFrom}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('range_to')}</t>
-  </si>
-  <si>
-    <t>${birthDateTo}</t>
-  </si>
-  <si>
-    <t>${description}</t>
-  </si>
-  <si>
-    <t>${homeAddress}</t>
-  </si>
-  <si>
-    <t>${msg.getProperty('Security Roles')}</t>
-  </si>
-  <si>
-    <t>${securityRoles}</t>
+    <t>${version}</t>
   </si>
 </sst>
 </file>
@@ -550,45 +448,6 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P1" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -599,45 +458,6 @@
       </c>
       <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -657,134 +477,77 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>